<commit_message>
delete and import prompts
</commit_message>
<xml_diff>
--- a/backend/prompts.xlsx
+++ b/backend/prompts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://version1-my.sharepoint.com/personal/s_vaishnavi_version1_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShettySh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3F8D3B9-FE1B-4246-8D65-B57CA51D0774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A874E5-18FC-4FB1-A319-379182ACB885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B5FDFEF5-92C6-4975-BAA6-4BCAB82C1AF7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{B5FDFEF5-92C6-4975-BAA6-4BCAB82C1AF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,18 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="72">
   <si>
-    <t xml:space="preserve">prompt title </t>
-  </si>
-  <si>
-    <t xml:space="preserve">prompt </t>
-  </si>
-  <si>
-    <t>department</t>
-  </si>
-  <si>
-    <t>task type</t>
-  </si>
-  <si>
     <t>Email Chain Summary</t>
   </si>
   <si>
@@ -403,9 +391,6 @@
 - How to close constructively</t>
   </si>
   <si>
-    <t xml:space="preserve">output format  </t>
-  </si>
-  <si>
     <t>template</t>
   </si>
   <si>
@@ -455,6 +440,21 @@
   </si>
   <si>
     <t>explain / teach</t>
+  </si>
+  <si>
+    <t>task_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output_format  </t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>prompt_text</t>
   </si>
 </sst>
 </file>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FE01A2-8B77-4ABD-8BE7-9759FE0187ED}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -846,427 +846,427 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
         <v>56</v>
-      </c>
-      <c r="E2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
         <v>60</v>
-      </c>
-      <c r="D11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" t="s">
         <v>62</v>
-      </c>
-      <c r="D13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
         <v>64</v>
       </c>
-      <c r="D18" t="s">
-        <v>69</v>
-      </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E24" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E25" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>